<commit_message>
Update sync and pdo APIs
</commit_message>
<xml_diff>
--- a/DesignDocument/CANOPEN Design Document.xlsx
+++ b/DesignDocument/CANOPEN Design Document.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A6DA9F-C24F-4336-82B8-13E50D766BCC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0FF20D-F390-4F04-ACB7-1B3EC6596909}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="664" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="664" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CANOPEN Frame Summary" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="122">
   <si>
     <t>选用标准帧，11位CAN ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -693,6 +693,10 @@
   </si>
   <si>
     <t>4.  Write 0x6000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不支持</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1878,6 +1882,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>157383</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>81207</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57EF5084-4043-4494-8CCF-FB570820AAFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7711440" y="22860"/>
+          <a:ext cx="5857143" cy="5666667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>290711</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>3365</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="图片 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C877539E-E6EE-4AF8-B85E-9034D70843B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7673340" y="5730240"/>
+          <a:ext cx="6028571" cy="3561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2553,6 +2645,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>303848</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>116274</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD41E3D8-6462-4923-A62D-87EB12426DB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4437529"/>
+          <a:ext cx="7619048" cy="2133333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53789</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>53789</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>490894</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>136612</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC2994F9-B6DE-42E7-A724-6EBF5FC4AD5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="53789" y="6687671"/>
+          <a:ext cx="8361905" cy="800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2564,7 +2744,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACE"/>
+        <a:sysClr val="window" lastClr="CEEACA"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2905,7 +3085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2982,8 +3162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4BA3B6-4718-494D-BF46-F69C4055E04A}">
   <dimension ref="A15:B39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3414,8 +3594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4E7A91-14D1-4B81-BE6E-FEF6AD56F741}">
   <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3941,10 +4121,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3064DAED-904E-4C29-A651-1714AB84003A}">
-  <dimension ref="A22:C23"/>
+  <dimension ref="A22:O40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q39" activeCellId="1" sqref="O40 Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3965,6 +4145,11 @@
         <v>113</v>
       </c>
     </row>
+    <row r="40" spans="15:15">
+      <c r="O40" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor change for sync and PDO
</commit_message>
<xml_diff>
--- a/DesignDocument/CANOPEN Design Document.xlsx
+++ b/DesignDocument/CANOPEN Design Document.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0FF20D-F390-4F04-ACB7-1B3EC6596909}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BBD612-1EC9-41CB-BCB6-5EB399D4706F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="664" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="664" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CANOPEN Frame Summary" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="123">
   <si>
     <t>选用标准帧，11位CAN ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -697,6 +697,10 @@
   </si>
   <si>
     <t>不支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Charger是同步发起者</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2733,6 +2737,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>8966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>284724</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>117470</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4353C818-F557-44E2-B7F1-C02E9717E269}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7897907"/>
+          <a:ext cx="8209524" cy="1542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3140,7 +3188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BB1251-4199-4195-B2FA-6BF22DC47CB4}">
   <dimension ref="L30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
@@ -3162,7 +3210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4BA3B6-4718-494D-BF46-F69C4055E04A}">
   <dimension ref="A15:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
@@ -4121,10 +4169,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3064DAED-904E-4C29-A651-1714AB84003A}">
-  <dimension ref="A22:O40"/>
+  <dimension ref="A22:O48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q39" activeCellId="1" sqref="O40 Q39"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T54" sqref="T54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4150,6 +4198,11 @@
         <v>121</v>
       </c>
     </row>
+    <row r="48" spans="15:15">
+      <c r="O48" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update some Critical documents
</commit_message>
<xml_diff>
--- a/DesignDocument/CANOPEN Design Document.xlsx
+++ b/DesignDocument/CANOPEN Design Document.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FC46B1-A191-4091-BDB6-ABB8DE5509EF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A904C30-DADB-4C81-A0B3-B8C26FE37002}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="664" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="664" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CANOPEN Frame Summary" sheetId="2" r:id="rId1"/>
     <sheet name="CAN Frame Description" sheetId="1" r:id="rId2"/>
     <sheet name="PDO remap" sheetId="3" r:id="rId3"/>
-    <sheet name="SDO" sheetId="4" r:id="rId4"/>
-    <sheet name="OD" sheetId="5" r:id="rId5"/>
-    <sheet name="Test Frame" sheetId="6" r:id="rId6"/>
-    <sheet name="NMT" sheetId="7" r:id="rId7"/>
-    <sheet name="SYNC" sheetId="8" r:id="rId8"/>
+    <sheet name="上位机测试" sheetId="9" r:id="rId4"/>
+    <sheet name="SDO" sheetId="4" r:id="rId5"/>
+    <sheet name="OD" sheetId="5" r:id="rId6"/>
+    <sheet name="Test Frame" sheetId="6" r:id="rId7"/>
+    <sheet name="NMT" sheetId="7" r:id="rId8"/>
+    <sheet name="SYNC" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Test Frame'!$A$1:$D$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Test Frame'!$A$1:$D$32</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1630,6 +1631,55 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>561371</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>37657</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECA9B444-318C-4A2C-9564-DD398FF696BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4828571" cy="3542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>51154</xdr:colOff>
       <xdr:row>13</xdr:row>
@@ -2025,7 +2075,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2074,7 +2124,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2607,7 +2657,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2840,7 +2890,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACE"/>
+        <a:sysClr val="window" lastClr="CEEACA"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -3236,8 +3286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BB1251-4199-4195-B2FA-6BF22DC47CB4}">
   <dimension ref="L29:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3260,6 +3310,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2846C52-A631-431A-AF2F-18EF13F35CFD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4BA3B6-4718-494D-BF46-F69C4055E04A}">
   <dimension ref="A15:B39"/>
   <sheetViews>
@@ -3289,7 +3355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFB222D-24EC-4E06-BB67-97ED9145197A}">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -3691,11 +3757,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4E7A91-14D1-4B81-BE6E-FEF6AD56F741}">
   <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -4204,7 +4270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683CFE21-8CB8-4AF6-A233-D3E15E306C08}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4220,12 +4286,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3064DAED-904E-4C29-A651-1714AB84003A}">
   <dimension ref="A22:O48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T54" sqref="T54"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>